<commit_message>
orders: added [mailboxes] and [order_params] to the xlsx export.
</commit_message>
<xml_diff>
--- a/htdocs/assets/orders.xlsx
+++ b/htdocs/assets/orders.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -94,6 +94,12 @@
     <t xml:space="preserve">Примечание</t>
   </si>
   <si>
+    <t xml:space="preserve">Дополнительные параметры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Адреса электронной почты</t>
+  </si>
+  <si>
     <t xml:space="preserve">Руководитель</t>
   </si>
   <si>
@@ -119,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
   </si>
 </sst>
 </file>
@@ -127,7 +139,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0"/>
@@ -386,18 +398,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V2" activeCellId="0" sqref="V2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,9 +435,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="5" width="14.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="5" width="13.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="5" width="14.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="41.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="67" min="26" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="3" width="41.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="67" min="28" style="6" width="8.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="68" style="7" width="8.5"/>
   </cols>
   <sheetData>
@@ -454,6 +466,8 @@
       <c r="W1" s="12"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
@@ -533,6 +547,12 @@
       <c r="Y2" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="Z2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="n">
@@ -584,37 +604,43 @@
         <v>16</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T3" s="17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U3" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="V3" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W3" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="Z3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
orders: added second page to the xlsx template (orders with products).
</commit_message>
<xml_diff>
--- a/htdocs/assets/orders.xlsx
+++ b/htdocs/assets/orders.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="products" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -131,6 +132,33 @@
   </si>
   <si>
     <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Продукт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Упак.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
   </si>
 </sst>
 </file>
@@ -378,11 +406,11 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -590,4 +618,251 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="U6" activeCellId="0" sqref="U6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="22.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="46.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="3" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="16.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="25.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="23.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="25.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="9.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="38.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="4" width="11.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="5" width="14.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="5" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="5" width="14.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="3" width="41.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="71" min="32" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="72" style="7" width="8.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="L2" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="M2" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="N2" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="O2" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="P2" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;KffffffСтраница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>